<commit_message>
data updated at 13 Dec 7PM
</commit_message>
<xml_diff>
--- a/Retailers Ledger/KALER.xlsx
+++ b/Retailers Ledger/KALER.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="3" activeTab="4"/>
+    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RAJA MOBILE CENTER-(661032976)" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="NAVEEN MOB CENTRE-(660903120)" sheetId="4" r:id="rId3"/>
     <sheet name="SANTOSH PUSTAK BHAN-(661063900)" sheetId="5" r:id="rId4"/>
     <sheet name="Glaxy Mobile Studio-(660587311)" sheetId="6" r:id="rId5"/>
+    <sheet name="NAVEEN RECHARGE CENT(661474491)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="18">
   <si>
     <t>RAJA MOBILE CENTER-(661032976)</t>
   </si>
@@ -70,17 +71,20 @@
   <si>
     <t>Glaxy Mobile and Digital Studio-(660587311)</t>
   </si>
+  <si>
+    <t>NAVEEN RECHARGE CENTRE(661474491)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -97,35 +101,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -136,37 +111,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -174,30 +118,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,7 +134,75 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,20 +215,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -268,25 +272,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,157 +428,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,11 +468,65 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,31 +550,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,50 +563,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -582,130 +586,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -725,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -743,7 +747,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2382,8 +2386,8 @@
   <sheetPr/>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -2642,4 +2646,243 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.14285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:5">
+      <c r="A4" s="5">
+        <v>44177</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2080</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6">
+        <f>IF(A4="","",E3+B4/1.04-C4)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:5">
+      <c r="A5" s="5"/>
+      <c r="E5" s="6" t="str">
+        <f t="shared" ref="E5:E23" si="0">IF(A5="","",E4+B5/1.04-C5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:5">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="5:5">
+      <c r="E10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="5:5">
+      <c r="E11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="5:5">
+      <c r="E12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="5:5">
+      <c r="E13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="5:5">
+      <c r="E14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="5:5">
+      <c r="E15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="5:5">
+      <c r="E16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="5:5">
+      <c r="E17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="5:5">
+      <c r="E18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="5:5">
+      <c r="E19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="5:5">
+      <c r="E20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="5:5">
+      <c r="E21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="5:5">
+      <c r="E22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="5:5">
+      <c r="E23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="5:5">
+      <c r="E24" s="6" t="str">
+        <f>IF(A24="","",E23+B24/1.04-C24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="5:5">
+      <c r="E25" s="6" t="str">
+        <f>IF(A25="","",E24+B25/1.04-C25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="1" spans="5:5">
+      <c r="E26" s="6" t="str">
+        <f>IF(A26="","",E25+B26/1.04-C26)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="5:5">
+      <c r="E27" s="6" t="str">
+        <f>IF(A27="","",E26+B27/1.04-C27)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>